<commit_message>
updates to data cleaning
</commit_message>
<xml_diff>
--- a/src/A-data-cleaning/data_received/data_20230120.xlsx
+++ b/src/A-data-cleaning/data_received/data_20230120.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgaythor\Documents\Teaching\orderly_training\src\A-data-cleaning\data_received\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5107338-5FC8-4A68-AC62-6341E3306CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18903F8A-6C94-436F-A213-555E6DAEBB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5273AEA4-57F6-43AA-8CCA-05F0B2D92416}"/>
   </bookViews>
@@ -182,11 +182,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,61 +510,61 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -573,33 +573,33 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="3"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -617,23 +617,23 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
@@ -644,7 +644,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B4">
@@ -655,7 +655,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B5">
@@ -666,7 +666,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B6">
@@ -677,7 +677,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B7">
@@ -688,7 +688,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B8">
@@ -699,7 +699,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B9">
@@ -710,7 +710,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B10">
@@ -721,7 +721,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B11">
@@ -732,7 +732,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B12">
@@ -743,7 +743,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B13">
@@ -754,7 +754,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B14">
@@ -765,7 +765,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B15">
@@ -776,7 +776,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B16">
@@ -787,7 +787,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B17">
@@ -798,7 +798,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B18">
@@ -809,7 +809,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B19">
@@ -820,7 +820,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B20">
@@ -831,7 +831,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B21">
@@ -842,7 +842,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B22">
@@ -853,7 +853,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B23">
@@ -864,7 +864,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B24">
@@ -875,18 +875,18 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B25">
         <v>53</v>
       </c>
       <c r="C25">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B26">

</xml_diff>

<commit_message>
tweaking the input data
</commit_message>
<xml_diff>
--- a/src/A-data-cleaning/data_received/data_20230120.xlsx
+++ b/src/A-data-cleaning/data_received/data_20230120.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgaythor\Documents\Teaching\orderly_training\src\A-data-cleaning\data_received\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18903F8A-6C94-436F-A213-555E6DAEBB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A748FF-9C05-42F5-9AE1-F28139E93240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5273AEA4-57F6-43AA-8CCA-05F0B2D92416}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{5273AEA4-57F6-43AA-8CCA-05F0B2D92416}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -617,7 +617,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
         <v>55</v>
       </c>
       <c r="C24">
-        <v>0.79</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -882,7 +882,7 @@
         <v>53</v>
       </c>
       <c r="C25">
-        <v>0.8</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -893,7 +893,7 @@
         <v>56</v>
       </c>
       <c r="C26">
-        <v>0.79</v>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding simple reportand tweaking data
</commit_message>
<xml_diff>
--- a/src/A-data-cleaning/data_received/data_20230120.xlsx
+++ b/src/A-data-cleaning/data_received/data_20230120.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgaythor\Documents\Teaching\orderly_training\src\A-data-cleaning\data_received\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A748FF-9C05-42F5-9AE1-F28139E93240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B6F2E7-3945-4547-9740-26867A852A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{5273AEA4-57F6-43AA-8CCA-05F0B2D92416}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{5273AEA4-57F6-43AA-8CCA-05F0B2D92416}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -57,12 +57,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>YF coverage</t>
-  </si>
-  <si>
-    <t>Measles coverage</t>
-  </si>
-  <si>
     <t>2022-01-03</t>
   </si>
   <si>
@@ -130,6 +124,12 @@
   </si>
   <si>
     <t>2000-04-01</t>
+  </si>
+  <si>
+    <t>GF coverage</t>
+  </si>
+  <si>
+    <t>BF coverage</t>
   </si>
 </sst>
 </file>
@@ -507,9 +507,9 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -521,7 +521,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4" s="2"/>
       <c r="C4" s="4" t="s">
         <v>0</v>
@@ -535,7 +535,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
       <c r="C5" s="4" t="s">
         <v>1</v>
@@ -549,7 +549,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
       <c r="C6" s="4" t="s">
         <v>2</v>
@@ -563,7 +563,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -575,7 +575,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" s="2"/>
       <c r="C8" s="4" t="s">
         <v>3</v>
@@ -589,7 +589,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -617,35 +617,35 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>65</v>
@@ -654,9 +654,9 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>64</v>
@@ -665,9 +665,9 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>67</v>
@@ -676,9 +676,9 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>67</v>
@@ -687,9 +687,9 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>64</v>
@@ -698,9 +698,9 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>65</v>
@@ -709,9 +709,9 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>68</v>
@@ -720,9 +720,9 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>69</v>
@@ -731,9 +731,9 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>66</v>
@@ -742,9 +742,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>64</v>
@@ -753,9 +753,9 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>62</v>
@@ -764,9 +764,9 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>61</v>
@@ -775,9 +775,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>63</v>
@@ -786,9 +786,9 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>60</v>
@@ -797,9 +797,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18">
         <v>58</v>
@@ -808,9 +808,9 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B19">
         <v>60</v>
@@ -819,9 +819,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B20">
         <v>59</v>
@@ -830,9 +830,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B21">
         <v>57</v>
@@ -841,9 +841,9 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22">
         <v>55</v>
@@ -852,9 +852,9 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B23">
         <v>56</v>
@@ -863,9 +863,9 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B24">
         <v>55</v>
@@ -874,9 +874,9 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B25">
         <v>53</v>
@@ -885,9 +885,9 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B26">
         <v>56</v>

</xml_diff>